<commit_message>
upload of midpoint fyp
</commit_message>
<xml_diff>
--- a/FYP - Documents/UnOffical Documents/Time Scale For FYP.xlsx
+++ b/FYP - Documents/UnOffical Documents/Time Scale For FYP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\co0ki\Documents\University Work\Year 3\FYP\UnOffical Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\co0ki\Documents\GitHub\Final-Year-Project\FYP - Documents\UnOffical Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB070DDC-07C8-4E9C-828D-0038E6732A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F16427-8B1B-4231-9207-782716DD6E1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18405" yWindow="0" windowWidth="19995" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="28800" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +144,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -448,11 +454,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -486,12 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
@@ -519,6 +541,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,55 +877,55 @@
   <dimension ref="B1:AC13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="8" width="3.140625" customWidth="1"/>
-    <col min="9" max="11" width="2.7109375" customWidth="1"/>
-    <col min="12" max="12" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="8" width="3.109375" customWidth="1"/>
+    <col min="9" max="11" width="2.6640625" customWidth="1"/>
+    <col min="12" max="12" width="2.88671875" customWidth="1"/>
     <col min="13" max="13" width="3" customWidth="1"/>
     <col min="14" max="26" width="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="1.28515625" customWidth="1"/>
-    <col min="28" max="28" width="2.85546875" customWidth="1"/>
-    <col min="29" max="29" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="1.33203125" customWidth="1"/>
+    <col min="28" max="28" width="2.88671875" customWidth="1"/>
+    <col min="29" max="29" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6"/>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="35"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="33"/>
     </row>
-    <row r="3" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
@@ -983,22 +1019,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+    <row r="4" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1011,27 +1047,27 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="19"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="24" t="s">
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -1044,27 +1080,27 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="19"/>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="26" t="s">
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1077,27 +1113,27 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="19"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="26" t="s">
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1111,27 +1147,27 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="3"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
@@ -1140,27 +1176,27 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="19"/>
     </row>
-    <row r="9" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -1169,22 +1205,22 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="19"/>
     </row>
-    <row r="10" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="4"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="40"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -1198,22 +1234,22 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="19"/>
     </row>
-    <row r="11" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
       <c r="O11" s="3"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -1227,22 +1263,22 @@
       <c r="Y11" s="17"/>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1256,22 +1292,22 @@
       <c r="Y12" s="18"/>
       <c r="Z12" s="19"/>
     </row>
-    <row r="13" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>

</xml_diff>